<commit_message>
Updated assignment and backlog
</commit_message>
<xml_diff>
--- a/Project 1/Product Backlog.xlsx
+++ b/Project 1/Product Backlog.xlsx
@@ -9,14 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog - Meeting 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint Backlog 1" sheetId="2" r:id="rId2"/>
     <sheet name="Product Backlog - Meeting 2" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint Backlog 2" sheetId="4" r:id="rId4"/>
-    <sheet name="Team Members" sheetId="7" r:id="rId5"/>
+    <sheet name="Sprint Backlog - Meeting 3" sheetId="8" r:id="rId5"/>
+    <sheet name="Sprint BackLog 3" sheetId="9" r:id="rId6"/>
+    <sheet name="Team Members" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -95,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
   <si>
     <t>As a hotel owner I want a payment details portal so that I can assist my customers</t>
   </si>
@@ -254,6 +256,30 @@
   </si>
   <si>
     <t>As a owner I want to support loyality points to that customers can redeem for a deal</t>
+  </si>
+  <si>
+    <t>As a customer I want to see my pervious bookings so that I can see what I paid ( compare prices)</t>
+  </si>
+  <si>
+    <t>As a customer I want to get an email notification of payment so that I can have proof of payment</t>
+  </si>
+  <si>
+    <t>As a hotel owner I want to see the resurant menu so that customers will know what food options there are</t>
+  </si>
+  <si>
+    <t>As a customer I want to have an option to book a meeting hall so that I can online book an event</t>
+  </si>
+  <si>
+    <t>As a hotel owner I want a special role so that I can have different access for different users ( admin/users)</t>
+  </si>
+  <si>
+    <t>As a hotel owner I want to implement a live chat for employees so that I can assist my customers in real time</t>
+  </si>
+  <si>
+    <t>As a customer I want to schedue an airport pickup so that I be picked up by the hotel airport shuttle</t>
+  </si>
+  <si>
+    <t>As a customer I want to re-schedue an airport pickup so that I be picked up by the hotel airport shuttle</t>
   </si>
 </sst>
 </file>
@@ -869,7 +895,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="B2:D18"/>
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1016,7 +1042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1030,6 +1056,177 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="97" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>

</xml_diff>